<commit_message>
Read metadata sheet from xlsx
</commit_message>
<xml_diff>
--- a/packages/lan/data/test_programs.xlsx
+++ b/packages/lan/data/test_programs.xlsx
@@ -5,10 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Tupaia User Survey Tonga RH" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tupaia User Survey Tonga RH" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Ignored" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,9 +22,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+  <si>
+    <t xml:space="preserve">programName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tamanu test suite program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">programCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test-program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev</t>
+  </si>
   <si>
     <t xml:space="preserve">code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">surveyType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">targetLocationId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">targetDepartmentId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-tonga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tupaia User Survey Tonga RH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">programs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-location-id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-department-id</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
@@ -346,8 +396,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -368,349 +422,443 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="19.25"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="86.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="247.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -724,4 +872,27 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update admin endpoint to use new importer
</commit_message>
<xml_diff>
--- a/packages/lan/data/test_programs.xlsx
+++ b/packages/lan/data/test_programs.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Tupaia User Survey Tonga RH" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Ignored" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Field types" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Tupaia User Survey Tonga RH" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Ignored" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="150">
   <si>
     <t xml:space="preserve">programName</t>
   </si>
@@ -60,6 +61,21 @@
     <t xml:space="preserve">visibility</t>
   </si>
   <si>
+    <t xml:space="preserve">Test-fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Field types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">referral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-location-id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-department-id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test-tonga</t>
   </si>
   <si>
@@ -69,12 +85,6 @@
     <t xml:space="preserve">programs</t>
   </si>
   <si>
-    <t xml:space="preserve">Test-location-id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test-department-id</t>
-  </si>
-  <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
@@ -117,12 +127,180 @@
     <t xml:space="preserve">detailLabel</t>
   </si>
   <si>
+    <t xml:space="preserve">Types_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FreeText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the patient’s name?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MultiSelect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SubmissionDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checkbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CalculatedQuestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConditionQuestion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arithmetic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SurveyLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SurveyAnswer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SurveyResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PatientData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EarlyTerminator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClinicalSupport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoriser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table lookup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autocomplete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types_27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo</t>
+  </si>
+  <si>
     <t xml:space="preserve">TamanuProgramsTest1</t>
   </si>
   <si>
-    <t xml:space="preserve">Instruction</t>
-  </si>
-  <si>
     <t xml:space="preserve">Please enter all data accurately to determine if this patient has risk factors for COVID-19</t>
   </si>
   <si>
@@ -138,9 +316,6 @@
     <t xml:space="preserve">TamanuProgramsTest3</t>
   </si>
   <si>
-    <t xml:space="preserve">Date</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date of survey</t>
   </si>
   <si>
@@ -150,9 +325,6 @@
     <t xml:space="preserve">TamanuProgramsTest4</t>
   </si>
   <si>
-    <t xml:space="preserve">FreeText</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name of user</t>
   </si>
   <si>
@@ -160,9 +332,6 @@
   </si>
   <si>
     <t xml:space="preserve">TamanuProgramsTest5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radio</t>
   </si>
   <si>
     <t xml:space="preserve">Position</t>
@@ -197,9 +366,6 @@
     <t xml:space="preserve">TamanuProgramsTest7</t>
   </si>
   <si>
-    <t xml:space="preserve">Binary</t>
-  </si>
-  <si>
     <t xml:space="preserve">Recent COVID-19 contact</t>
   </si>
   <si>
@@ -288,9 +454,6 @@
   </si>
   <si>
     <t xml:space="preserve">TamanuProgramsTest17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Checkbox</t>
   </si>
   <si>
     <t xml:space="preserve">COVID risk: Immunocompromised reason</t>
@@ -426,10 +589,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -483,7 +646,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
@@ -503,8 +666,28 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -521,10 +704,314 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:O1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.48"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -540,325 +1027,325 @@
         <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>35</v>
+        <v>94</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="247.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>45</v>
+        <v>102</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>48</v>
+        <v>104</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>49</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>51</v>
+        <v>107</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>61</v>
+        <v>116</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>64</v>
+        <v>119</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>65</v>
+        <v>120</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>67</v>
+        <v>122</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>69</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>73</v>
+        <v>128</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>74</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>77</v>
+        <v>132</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>79</v>
+        <v>134</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>80</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>83</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>86</v>
+        <v>140</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>88</v>
+        <v>142</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -874,14 +1361,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update invalid test survey data
</commit_message>
<xml_diff>
--- a/packages/lan/data/test_programs.xlsx
+++ b/packages/lan/data/test_programs.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Metadata" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Field types" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Tupaia User Survey Tonga RH" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Samoa PEN Referral Example" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Ignored" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="169">
   <si>
     <t xml:space="preserve">programName</t>
   </si>
@@ -79,18 +79,21 @@
     <t xml:space="preserve">Test-department-id</t>
   </si>
   <si>
+    <t xml:space="preserve">hidden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test-tonga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samoa PEN Referral Example</t>
+  </si>
+  <si>
+    <t xml:space="preserve">programs</t>
+  </si>
+  <si>
     <t xml:space="preserve">publish</t>
   </si>
   <si>
-    <t xml:space="preserve">Test-tonga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tupaia User Survey Tonga RH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">programs</t>
-  </si>
-  <si>
     <t xml:space="preserve">type</t>
   </si>
   <si>
@@ -304,192 +307,229 @@
     <t xml:space="preserve">Photo</t>
   </si>
   <si>
-    <t xml:space="preserve">TamanuProgramsTest1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter all data accurately to determine if this patient has risk factors for COVID-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please ensure all basic patient demographics including Sex and Date of Birth have been updated in the Patient Details section. These do not need to be entered here.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Date of survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter today's date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is your name? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">What is your position title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nurse
-Nurse Aid
-Midwife
-Doctor
-Pharmacy support
-Pharmacist
-Ministry of Health
-Administrative
-HIS
-Project Staff
-Development Partner/Donor
-Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patient current village</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which village is the patient currently living in?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recent COVID-19 contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the patient had recent contact with a confirmed COVID-19 patient?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recent international travel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the patient recently travelled internationally?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country of international travel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which country/countries has the patient travelled to in the last 21 days?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Close contact with international travel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has the patient has close contact with a recent international traveller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;70 years of age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the patient &gt;70 years of age</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does the patient have any of the following conditions:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID risk: CVD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cardiovascular disease</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID risk: Diabetes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diabetes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID risk: Auto-immune condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto-immune condition such as Lupus or MS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID risk: Immunocompromised</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is the patient immuno-compromised for any reason?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID risk: Immunocompromised reason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is this due to an ongoing condition or current drug therapy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ongoing Condition, Drug Therapy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest14: Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID risk: Cancer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does the patient have cancer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TamanuProgramsTest19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COVID risk: Terminal condition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Does the patient have a seriously life-threatening or terminal illness</t>
+    <t xml:space="preserve">calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referral date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referred to</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEN Fa'aSamoa screening results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ "source": "program-samoancdscreening-penfaasamoa" }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referral Criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mafuaaga e tatau ai ona alu i le falemai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heart disease warning signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auga o le ma’Ifatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-06"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stroke warning signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stroke warning signs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auga o le stroke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-07"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diabetes warning signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auga o le ma'Isuka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-08"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heart disease/stroke/diabetes symptoms?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does the individual have heart disease/stroke/diabetes symptoms?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auga o le ma’Ifatu/stroke/ma'lsuka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Heart disease (ma'lfatu)": "Heart disease (ma'lfatu)", "Stroke (stroke)": "Stroke (stroke)", "Diabetes (ma'lsuka)": "Diabetes (ma'lsuka)"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous experience of cardiovascular disease?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"Never assessed before": "Never assessed before", "No recent visit and/or medications run out": "No recent visit and/or medications run out"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random glucose 1st reading (mmol/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fua ole Suka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-34"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random glucose 2nd reading (mmol/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-35"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High blood glucose (&gt;11mmol/L)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maualuga le suka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average systolic blood pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-29"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average diastolic blood pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-32"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High blood pressure (&gt;140 (systolic) /90 (diastolic) mmHg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select box if high blood pressure (&gt;140 (systolic) /90 (diastolic) mmHg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maualuga le toto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHO/ISH risk level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High WHO/ISH risk (≥30%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select box if high WHO/ISH risk (≥30%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maualuga le avanoa e ono mauaai I le ma’Ifatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenatal check ups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual has had antenatal check ups for this pregnancy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ua siaki lau to e se fomai poo se tausi soifua?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"SamNCD-39": "Yes (I'oe)"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"source": "SamNCD-41"}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antenatal checkup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select box if individual has NOT had antenatal check ups for this pregnancy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other reason for review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Briefly explain why review is requested if different from above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faamatala le mafuaga pe afai e ese mai I mafuaaga ua taua I luga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamPENRef-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Referral completed by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepa faatumuina e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"column": "displayName"}</t>
   </si>
 </sst>
 </file>
@@ -598,14 +638,14 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="19.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="19.27"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,7 +734,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -721,7 +761,7 @@
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.47"/>
@@ -732,273 +772,273 @@
         <v>7</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1019,10 +1059,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1033,334 +1073,658 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="86.37"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="G1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="D2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="B4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="D4" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="247.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="D5" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="B7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+    <row r="8" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="B8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="204.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="B9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="F9" s="1"/>
+      <c r="G9" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="228.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="B10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="D10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="D11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="B12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="D12" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="B13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="D13" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="0" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="B14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="D14" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="B15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="D15" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="B16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="D16" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="K18" s="0" t="s">
+      <c r="E16" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="0" t="s">
+      <c r="B17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D17" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="B18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="0" t="s">
+      <c r="D18" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="E18" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" customFormat="false" ht="97" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1383,7 +1747,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>